<commit_message>
modify the pattern5 and pattern6
</commit_message>
<xml_diff>
--- a/p2-plus5.xlsx
+++ b/p2-plus5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\plus5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="121">
   <si>
     <t>Table 1</t>
   </si>
@@ -46,20 +46,12 @@
   </si>
   <si>
     <t>Patch Arch Pattern</t>
-  </si>
-  <si>
-    <t>Corn,Lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>all files added new features about Event Bus Service</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>pattern6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>remove the file profile_operation and its reference</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -68,10 +60,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>modify the leading file IUMap's method and modify its reference in the subordinate files</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -80,10 +68,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>corn (with connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>add new features in all the files</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -100,10 +84,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5 (Lambda,anchor?)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>part of  files are architecturally connected (2Corn:2lambda:1test)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -180,14 +160,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>corn (without connection), Lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>corn (with connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>add first, second and third operation in the leading files and similar code in the other files</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -208,10 +180,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern6,Upsilon</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern6: AbstractPage_c.java-&gt;ImportFromInstallationWizard_c.java, Upsilon: AbstractPage_c.java.ProvUIMessage.java-&gt;AutomaticUpdateScheduler.java</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -240,10 +208,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5,Lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern5: ProvisioningListener.java-&gt;ArtifactRepositoryManager.java,MetadataRepositoryManager.java, RepositoryEvent.java-&gt;UpdateSiteMetadataRepository.java, Lambda: SiteModel.java-&gt;DefaultSiteParser.java</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -264,19 +228,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5,Lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern5: IProfileRegistry.java-&gt;DirectorApplication, Lambda:  Iprofile.java-&gt;ProfileSnapshot.java, ProfileSynchronizer</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Lambda: Add the field in the leading file and modified the assoicated files. Pattern5: add the reference code in the subordinate files</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Upsilon,Lambda</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -308,10 +264,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5,Corn(with similar connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern5 (Corn): SecureXMLUtil.java-&gt;MirrorSelector.java, DirectoryParser.java, IUDeserializer.java, FeatureManifestParser.java,ProductFile.java, ConfigurationParser.java,UpdateManagerCompatibility.java,CategoryParser.java,DefaultSiteParser.java,DigestParser.java :</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -332,15 +284,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Refactor the two leading files and append several dependencies </t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Corn (with connection)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -377,30 +321,14 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>The reference about version in all the files are removed</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Corn (with connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pattern5 (external dependency),Corn (with connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>All the files are import same dependency and are patched similar code</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5,Lambda</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Lambda:ParameterizedProvisioningAction.java-&gt;InstructionParser.java ,Phase.java-&gt;PhaseSet.java, Pattern5: DebugHelper.java-&gt; SimpleProfileRegistry.java, Engine.java, EngineSession.java</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -428,18 +356,6 @@
     <t>all the files</t>
   </si>
   <si>
-    <t>all the files</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>all the files are added the same method invocation</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pattern5,Lambda,Corn (with connection)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern5:IUColumnConfig.java-&gt;AvailableIUsPage.java,ResolutionResultsWizardPage.java,ResolutionStatusPage.java,SelectableIUsPage.java,AcceptLicensesWizardPage.java,SelectableIUsPage.java, ProvisioningOperationWizard.java-&gt;ProvisioningWizardDialog.java Lambda:ILayoutConstants.java-&gt;ResolutionResultsWizardPage.java,AvailableIUsPage.java,ResolutionStatusPage.java,ResolutionResultsWizardPage.java,AcceptLicensesWizardPage.java Corn: ProvisioningWizardPage.java,ResolutionResultsWizardPage.java,ResolutionStatusPage.java,AcceptLicensesWizardPage.java</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -456,15 +372,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Pattern5: three files are added same dependencies</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pattern5:ProvUIMessages.java-&gt; IUViewQueryContext.java, AvailableIUWrapper.java, QueriedElementWrapper.java Corn: AvailableIUsPage.java, AvailableIUGroup.java</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -545,10 +453,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Pattern5: ProvisioningSession.java-&gt;MetadataRepositoryElementWrapper.java, ArtifactRepositoryElementWrapper.java ProfileSnapshots.java Pattern6: ProvisioningUI.java-&gt; MetadataRepositoryElementWrapper.java, ArtifactRepositoryElementWrapper.java , QueriedElementWrapper.java , ArtifactRepositoryElement.java ,ProvUIProvisioningListener.java </t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -565,15 +469,79 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>Pattern5: EquinoxBundlesState.java, EquinoxFwConfigFileParser.java, EquinoxManipulatorImpl.java, AbstractFwkAdminTest.java, NoConfigurationValueInEclipseIni.java, NoRenamingLauncherIni.java, OSGiVersionChange.java, RemovingABundle.java, RemovingAllBundles.java. RenamingLauncherIni.java, SimpleConfiguratorComingAndGoing.java, SimpleBundlesState.java, Utils.java, ConfiguratorManipulator.java, BundlesState.java, ConfigData.java, Manipulator.java, /EclipseInstallGeneratorInfoProvider.java, Generator.java, GeneratorBundleInfo.java, DataLoader.java, GeneratorBundleInfo.java, IProductDescriptor.java, ProductFile.java, BundlesAction.java, ConfigAdvice.java, ConfigCUsAction.java, IConfigAdvice.java, ProductFileAdvice.java. EclipseMarkSetProvider.java, LazyManipulator.java, PlatformConfigurationWrapper.java , SourceManipulator.java, WhatIsRunning.java,  InstallBundleAction.java, MarkStartedAction.java, SetStartLevelAction.java, UninstallBundleAction.java,</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Pattern5: most of the files are imported same dependendencies </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pattern5:ProvUIMessages.java-&gt; IUViewQueryContext.java, AvailableIUWrapper.java, QueriedElementWrapper.java Corn: AvailableIUsPage.java, AvailableIUGroup.java</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>all the files</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>all the files impleme the same method invocation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn (though connection)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lambda</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn (though connection)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <t>Corn,Pattern5</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Pattern5: EquinoxBundlesState.java, EquinoxFwConfigFileParser.java, EquinoxManipulatorImpl.java, AbstractFwkAdminTest.java, NoConfigurationValueInEclipseIni.java, NoRenamingLauncherIni.java, OSGiVersionChange.java, RemovingABundle.java, RemovingAllBundles.java. RenamingLauncherIni.java, SimpleConfiguratorComingAndGoing.java, SimpleBundlesState.java, Utils.java, ConfiguratorManipulator.java, BundlesState.java, ConfigData.java, Manipulator.java, /EclipseInstallGeneratorInfoProvider.java, Generator.java, GeneratorBundleInfo.java, DataLoader.java, GeneratorBundleInfo.java, IProductDescriptor.java, ProductFile.java, BundlesAction.java, ConfigAdvice.java, ConfigCUsAction.java, IConfigAdvice.java, ProductFileAdvice.java. EclipseMarkSetProvider.java, LazyManipulator.java, PlatformConfigurationWrapper.java , SourceManipulator.java, WhatIsRunning.java,  InstallBundleAction.java, MarkStartedAction.java, SetStartLevelAction.java, UninstallBundleAction.java,</t>
+    <t>Corn,Pattern5,Pattern6</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Pattern5: most of the files are imported same dependendencies </t>
+    <t>Lambda,Pattern5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lambda,Corn (though connection),Pattern5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn (though connection),Pattern5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn,Pattern6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lambda,Upsilon</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corn(though connection),Pattern5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upsilon,Pattern6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lambda,Corn</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lambda,Pattern6</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -2169,7 +2137,7 @@
   <dimension ref="A1:IV454"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G450" sqref="G450"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2180,7 +2148,7 @@
     <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="52.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46" style="1" customWidth="1"/>
     <col min="8" max="8" width="26" style="1" customWidth="1"/>
     <col min="9" max="256" width="8.28515625" style="1" customWidth="1"/>
   </cols>
@@ -2320,13 +2288,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2526,13 +2494,13 @@
         <v>3</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2732,11 +2700,11 @@
         <v>4</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -2936,13 +2904,13 @@
         <v>5</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3142,13 +3110,13 @@
         <v>5</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3348,13 +3316,13 @@
         <v>5</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3554,13 +3522,13 @@
         <v>6</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3760,13 +3728,13 @@
         <v>6</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G77" s="12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H77" s="12" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -3966,13 +3934,13 @@
         <v>6</v>
       </c>
       <c r="F87" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G87" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H87" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -4172,13 +4140,13 @@
         <v>7</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G97" s="12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H97" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -4378,13 +4346,13 @@
         <v>7</v>
       </c>
       <c r="F107" s="12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H107" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -4584,13 +4552,13 @@
         <v>7</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G117" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -4790,13 +4758,13 @@
         <v>8</v>
       </c>
       <c r="F127" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G127" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H127" s="12" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -4996,13 +4964,13 @@
         <v>8</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G137" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H137" s="12" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -5202,13 +5170,13 @@
         <v>8</v>
       </c>
       <c r="F147" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G147" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H147" s="12" t="s">
-        <v>42</v>
+        <v>119</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -5408,13 +5376,13 @@
         <v>9</v>
       </c>
       <c r="F157" s="18" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G157" s="18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H157" s="18" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -5614,13 +5582,13 @@
         <v>9</v>
       </c>
       <c r="F167" s="12" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G167" s="12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H167" s="12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -5820,13 +5788,13 @@
         <v>10</v>
       </c>
       <c r="F177" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G177" s="12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H177" s="12" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
     </row>
     <row r="178" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6026,13 +5994,13 @@
         <v>10</v>
       </c>
       <c r="F187" s="15" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G187" s="15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="H187" s="15" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6232,13 +6200,13 @@
         <v>11</v>
       </c>
       <c r="F197" s="12" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G197" s="12" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H197" s="12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6455,13 +6423,13 @@
         <v>11</v>
       </c>
       <c r="F208" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="G208" s="12" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H208" s="12" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
     </row>
     <row r="209" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6661,13 +6629,13 @@
         <v>12</v>
       </c>
       <c r="F218" s="12" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G218" s="12" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H218" s="12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -6867,13 +6835,13 @@
         <v>13</v>
       </c>
       <c r="F228" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G228" s="12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -7073,13 +7041,13 @@
         <v>13</v>
       </c>
       <c r="F238" s="12" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G238" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H238" s="16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -7279,13 +7247,13 @@
         <v>14</v>
       </c>
       <c r="F248" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G248" s="12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H248" s="12" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -7485,13 +7453,13 @@
         <v>14</v>
       </c>
       <c r="F258" s="12" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="G258" s="12" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="H258" s="12" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="259" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -7691,13 +7659,13 @@
         <v>16</v>
       </c>
       <c r="F268" s="12" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G268" s="12" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="H268" s="12" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="269" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -7897,13 +7865,13 @@
         <v>17</v>
       </c>
       <c r="F278" s="12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G278" s="12" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H278" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="279" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -8103,13 +8071,13 @@
         <v>19</v>
       </c>
       <c r="F288" s="12" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G288" s="19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="H288" s="12" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
     </row>
     <row r="289" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -8306,13 +8274,13 @@
         <v>21</v>
       </c>
       <c r="F298" s="12" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G298" s="12" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="H298" s="12" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="299" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -8512,13 +8480,13 @@
         <v>22</v>
       </c>
       <c r="F308" s="12" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="G308" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H308" s="12" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="309" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -8718,13 +8686,13 @@
         <v>23</v>
       </c>
       <c r="F318" s="12" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="G318" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="H318" s="12" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="319" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -8924,13 +8892,13 @@
         <v>25</v>
       </c>
       <c r="F328" s="12" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="G328" s="12" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="H328" s="12" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="329" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -9110,13 +9078,13 @@
         <v>27</v>
       </c>
       <c r="F337" s="12" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G337" s="12" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="H337" s="12" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="338" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -9316,13 +9284,13 @@
         <v>29</v>
       </c>
       <c r="F347" s="12" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="G347" s="12" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="H347" s="12" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="348" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -9522,13 +9490,13 @@
         <v>35</v>
       </c>
       <c r="F357" s="25" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="G357" s="25" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="H357" s="25" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="358" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -9728,13 +9696,13 @@
         <v>39</v>
       </c>
       <c r="F367" s="12" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G367" s="12" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="H367" s="12" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="368" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -9934,13 +9902,13 @@
         <v>42</v>
       </c>
       <c r="F377" s="12" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="G377" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H377" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="378" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -10160,13 +10128,13 @@
         <v>48</v>
       </c>
       <c r="F388" s="12" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="G388" s="12" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="H388" s="12" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="389" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -10346,13 +10314,13 @@
         <v>53</v>
       </c>
       <c r="F397" s="12" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G397" s="12" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="H397" s="12" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="398" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -10552,13 +10520,13 @@
         <v>59</v>
       </c>
       <c r="F407" s="12" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="G407" s="16" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="H407" s="12" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="408" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -10758,11 +10726,11 @@
         <v>65</v>
       </c>
       <c r="F417" s="26" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="G417" s="22"/>
       <c r="H417" s="26" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="418" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -10962,13 +10930,13 @@
         <v>75</v>
       </c>
       <c r="F427" s="12" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="G427" s="12" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="H427" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="428" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -11168,13 +11136,13 @@
         <v>107</v>
       </c>
       <c r="F437" s="12" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="G437" s="12" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="H437" s="12" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="438" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -11374,13 +11342,13 @@
         <v>144</v>
       </c>
       <c r="F447" s="12" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="G447" s="12" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="H447" s="12" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="448" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -11440,13 +11408,13 @@
         <v>170</v>
       </c>
       <c r="F450" s="12" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="G450" s="12" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="H450" s="12" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="451" spans="1:8" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>